<commit_message>
restore the Logos and fix booking nights
</commit_message>
<xml_diff>
--- a/Lynx Apartment Tracker.xlsx
+++ b/Lynx Apartment Tracker.xlsx
@@ -2411,7 +2411,7 @@
         <v>46049</v>
       </c>
       <c r="B25" s="19" t="n">
-        <v>46063</v>
+        <v>46077</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -2453,7 +2453,7 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="M25" t="n">
         <v>1054.84</v>

</xml_diff>